<commit_message>
Fix path and update Excel
</commit_message>
<xml_diff>
--- a/Gas storages.xlsx
+++ b/Gas storages.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gvaps1\USR6\CHGE\desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gvaps1\USR6\CHGE\desktop\EUA dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BAA0A3-20DA-4CAE-880F-30CE49ED3064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C897D1-F965-4121-8954-95EB7CB5C8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F907BD33-5E94-4CC9-9082-BD4BC09FA10B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F907BD33-5E94-4CC9-9082-BD4BC09FA10B}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks" sheetId="1" r:id="rId1"/>
@@ -202,40 +202,40 @@
         <stp>PX_LAST</stp>
         <tr r="C5" s="2"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp t="s">
+        <v>Last Price</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[Gas storages.xlsx]Stocks!R5C4</stp>
         <stp>PX_LAST</stp>
         <tr r="D5" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp t="s">
+        <v>Last Price</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[Gas storages.xlsx]Stocks!R5C5</stp>
         <stp>PX_LAST</stp>
         <tr r="E5" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp t="s">
+        <v>Last Price</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[Gas storages.xlsx]Stocks!R5C6</stp>
         <stp>PX_LAST</stp>
         <tr r="F5" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp t="s">
+        <v>Last Price</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[Gas storages.xlsx]Stocks!R5C2</stp>
         <stp>PX_LAST</stp>
         <tr r="B5" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp t="s">
+        <v>Last Price</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[Gas storages.xlsx]Stocks!R5C3</stp>
@@ -254,11 +254,9 @@
         <v>#N/A</v>
         <stp/>
         <stp>BDH|5828156284080324637</stp>
+        <tr r="A7" s="2"/>
         <tr r="A7" s="3"/>
-        <tr r="A7" s="2"/>
       </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
       <tp t="e">
         <v>#N/A</v>
         <stp/>
@@ -281,24 +279,24 @@
       </tp>
     </main>
     <main first="bloomberg.rtd">
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[Gas storages.xlsx]Correl EUA vs stocks!R5C4</stp>
         <stp>PX_LAST</stp>
         <tr r="D5" s="3"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[Gas storages.xlsx]Correl EUA vs stocks!R5C3</stp>
         <stp>PX_LAST</stp>
         <tr r="C5" s="3"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[Gas storages.xlsx]Correl EUA vs stocks!R5C2</stp>
@@ -627,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3900AD71-E3B4-44B6-951D-A8605D5D6C7F}">
-  <dimension ref="A1:F1449"/>
+  <dimension ref="A1:F1452"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A1416" workbookViewId="0">
+      <selection activeCell="E1437" sqref="E1437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,26 +732,26 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=1443")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=1446")</f>
         <v>43831</v>
       </c>
       <c r="B7">
         <v>990.32669999999996</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1443")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1446")</f>
         <v>3192</v>
       </c>
       <c r="D7">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1443")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1446")</f>
         <v>11.5663</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1443")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1446")</f>
         <v>233.00030000000001</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1443")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1446")</f>
         <v>107.5916</v>
       </c>
     </row>
@@ -28302,7 +28300,7 @@
         <v>45761</v>
       </c>
       <c r="B1385">
-        <v>404.54070000000002</v>
+        <v>404.5437</v>
       </c>
       <c r="C1385">
         <v>1846</v>
@@ -28322,7 +28320,7 @@
         <v>45762</v>
       </c>
       <c r="B1386">
-        <v>406.40789999999998</v>
+        <v>406.41199999999998</v>
       </c>
       <c r="C1386">
         <v>1846</v>
@@ -28342,7 +28340,7 @@
         <v>45763</v>
       </c>
       <c r="B1387">
-        <v>407.87560000000002</v>
+        <v>407.8809</v>
       </c>
       <c r="C1387">
         <v>1846</v>
@@ -28362,7 +28360,7 @@
         <v>45764</v>
       </c>
       <c r="B1388">
-        <v>409.55529999999999</v>
+        <v>409.5607</v>
       </c>
       <c r="C1388">
         <v>1846</v>
@@ -28382,7 +28380,7 @@
         <v>45765</v>
       </c>
       <c r="B1389">
-        <v>411.80399999999997</v>
+        <v>411.80950000000001</v>
       </c>
       <c r="C1389">
         <v>1934</v>
@@ -28402,7 +28400,7 @@
         <v>45768</v>
       </c>
       <c r="B1390">
-        <v>421.65809999999999</v>
+        <v>421.66370000000001</v>
       </c>
       <c r="C1390">
         <v>1934</v>
@@ -28422,7 +28420,7 @@
         <v>45769</v>
       </c>
       <c r="B1391">
-        <v>424.07010000000002</v>
+        <v>424.07569999999998</v>
       </c>
       <c r="C1391">
         <v>1934</v>
@@ -28442,7 +28440,7 @@
         <v>45770</v>
       </c>
       <c r="B1392">
-        <v>426.29649999999998</v>
+        <v>426.30220000000003</v>
       </c>
       <c r="C1392">
         <v>1934</v>
@@ -28462,7 +28460,7 @@
         <v>45771</v>
       </c>
       <c r="B1393">
-        <v>428.35930000000002</v>
+        <v>428.36500000000001</v>
       </c>
       <c r="C1393">
         <v>1934</v>
@@ -28482,7 +28480,7 @@
         <v>45772</v>
       </c>
       <c r="B1394">
-        <v>430.84730000000002</v>
+        <v>430.85309999999998</v>
       </c>
       <c r="C1394">
         <v>2041</v>
@@ -28502,7 +28500,7 @@
         <v>45775</v>
       </c>
       <c r="B1395">
-        <v>440.10070000000002</v>
+        <v>440.10649999999998</v>
       </c>
       <c r="C1395">
         <v>2041</v>
@@ -28522,7 +28520,7 @@
         <v>45776</v>
       </c>
       <c r="B1396">
-        <v>443.04640000000001</v>
+        <v>443.0523</v>
       </c>
       <c r="C1396">
         <v>2041</v>
@@ -28542,7 +28540,7 @@
         <v>45777</v>
       </c>
       <c r="B1397">
-        <v>446.47210000000001</v>
+        <v>446.47800000000001</v>
       </c>
       <c r="C1397">
         <v>2041</v>
@@ -28562,7 +28560,7 @@
         <v>45778</v>
       </c>
       <c r="B1398">
-        <v>451.053</v>
+        <v>451.05889999999999</v>
       </c>
       <c r="C1398">
         <v>2041</v>
@@ -28582,7 +28580,7 @@
         <v>45779</v>
       </c>
       <c r="B1399">
-        <v>455.55020000000002</v>
+        <v>455.55619999999999</v>
       </c>
       <c r="C1399">
         <v>2145</v>
@@ -28602,7 +28600,7 @@
         <v>45782</v>
       </c>
       <c r="B1400">
-        <v>468.02960000000002</v>
+        <v>468.03570000000002</v>
       </c>
       <c r="C1400">
         <v>2145</v>
@@ -28622,7 +28620,7 @@
         <v>45783</v>
       </c>
       <c r="B1401">
-        <v>470.53550000000001</v>
+        <v>470.54169999999999</v>
       </c>
       <c r="C1401">
         <v>2145</v>
@@ -28642,7 +28640,7 @@
         <v>45784</v>
       </c>
       <c r="B1402">
-        <v>472.83420000000001</v>
+        <v>472.84039999999999</v>
       </c>
       <c r="C1402">
         <v>2145</v>
@@ -29462,7 +29460,7 @@
         <v>45841</v>
       </c>
       <c r="B1443">
-        <v>676.88549999999998</v>
+        <v>676.89869999999996</v>
       </c>
       <c r="C1443">
         <v>2953</v>
@@ -29482,7 +29480,7 @@
         <v>45842</v>
       </c>
       <c r="B1444">
-        <v>680.06650000000002</v>
+        <v>680.10260000000005</v>
       </c>
       <c r="C1444">
         <v>3006</v>
@@ -29502,7 +29500,7 @@
         <v>45845</v>
       </c>
       <c r="B1445">
-        <v>694.74350000000004</v>
+        <v>694.77970000000005</v>
       </c>
       <c r="C1445">
         <v>3006</v>
@@ -29522,7 +29520,7 @@
         <v>45846</v>
       </c>
       <c r="B1446">
-        <v>698.20519999999999</v>
+        <v>698.24159999999995</v>
       </c>
       <c r="C1446">
         <v>3006</v>
@@ -29542,7 +29540,7 @@
         <v>45847</v>
       </c>
       <c r="B1447">
-        <v>702.5385</v>
+        <v>698.49390000000005</v>
       </c>
       <c r="C1447">
         <v>3006</v>
@@ -29551,10 +29549,10 @@
         <v>2.7158000000000002</v>
       </c>
       <c r="E1447">
-        <v>136.46639999999999</v>
+        <v>132.3784</v>
       </c>
       <c r="F1447">
-        <v>72.887100000000004</v>
+        <v>72.894099999999995</v>
       </c>
     </row>
     <row r="1448" spans="1:6" x14ac:dyDescent="0.25">
@@ -29562,7 +29560,7 @@
         <v>45848</v>
       </c>
       <c r="B1448">
-        <v>702.5385</v>
+        <v>701.80799999999999</v>
       </c>
       <c r="C1448">
         <v>3006</v>
@@ -29571,10 +29569,10 @@
         <v>2.7158000000000002</v>
       </c>
       <c r="E1448">
-        <v>136.46639999999999</v>
+        <v>133.46770000000001</v>
       </c>
       <c r="F1448">
-        <v>72.887100000000004</v>
+        <v>73.413899999999998</v>
       </c>
     </row>
     <row r="1449" spans="1:6" x14ac:dyDescent="0.25">
@@ -29582,7 +29580,7 @@
         <v>45849</v>
       </c>
       <c r="B1449">
-        <v>702.5385</v>
+        <v>705.46040000000005</v>
       </c>
       <c r="C1449">
         <v>3006</v>
@@ -29591,10 +29589,70 @@
         <v>2.7158000000000002</v>
       </c>
       <c r="E1449">
-        <v>136.46639999999999</v>
+        <v>134.36760000000001</v>
       </c>
       <c r="F1449">
-        <v>72.887100000000004</v>
+        <v>73.945400000000006</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1450" s="2">
+        <v>45852</v>
+      </c>
+      <c r="B1450">
+        <v>717.10310000000004</v>
+      </c>
+      <c r="C1450">
+        <v>3006</v>
+      </c>
+      <c r="D1450">
+        <v>2.8188</v>
+      </c>
+      <c r="E1450">
+        <v>137.4263</v>
+      </c>
+      <c r="F1450">
+        <v>75.330100000000002</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1451" s="2">
+        <v>45853</v>
+      </c>
+      <c r="B1451">
+        <v>717.10310000000004</v>
+      </c>
+      <c r="C1451">
+        <v>3006</v>
+      </c>
+      <c r="D1451">
+        <v>2.8188</v>
+      </c>
+      <c r="E1451">
+        <v>137.4263</v>
+      </c>
+      <c r="F1451">
+        <v>75.330100000000002</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1452" s="2">
+        <v>45854</v>
+      </c>
+      <c r="B1452">
+        <v>717.10310000000004</v>
+      </c>
+      <c r="C1452">
+        <v>3006</v>
+      </c>
+      <c r="D1452">
+        <v>2.8188</v>
+      </c>
+      <c r="E1452">
+        <v>137.4263</v>
+      </c>
+      <c r="F1452">
+        <v>75.330100000000002</v>
       </c>
     </row>
   </sheetData>
@@ -29606,8 +29664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CC2F69-7C8C-4154-8046-9289F76718B0}">
   <dimension ref="A1:C1190"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A1103" workbookViewId="0">
+      <selection activeCell="H1182" sqref="H1182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42682,7 +42740,7 @@
         <v>71.13</v>
       </c>
       <c r="C1190">
-        <v>34.659999999999997</v>
+        <v>34.975000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -42694,8 +42752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA1694F-2CC7-4C25-BDC0-AC1855FCDAD5}">
   <dimension ref="A1:D1392"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update gas storage data
</commit_message>
<xml_diff>
--- a/Gas storages.xlsx
+++ b/Gas storages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gvaps1\USR6\CHGE\desktop\EUA dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0113F744-5E5D-4711-8C58-CAC4B19B6789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69DC755-AD3B-4F33-8028-84BC7992DDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F907BD33-5E94-4CC9-9082-BD4BC09FA10B}"/>
   </bookViews>
@@ -623,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3900AD71-E3B4-44B6-951D-A8605D5D6C7F}">
-  <dimension ref="A1:F1455"/>
+  <dimension ref="A1:F1459"/>
   <sheetViews>
-    <sheetView topLeftCell="A1416" workbookViewId="0">
-      <selection activeCell="F1429" sqref="F1429"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,26 +730,26 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=1449")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=1453")</f>
         <v>43831</v>
       </c>
       <c r="B7">
         <v>990.32669999999996</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1449")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1453")</f>
         <v>3192</v>
       </c>
       <c r="D7">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1449")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1453")</f>
         <v>11.5663</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1449")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1453")</f>
         <v>233.00030000000001</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1449")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1453")</f>
         <v>107.5916</v>
       </c>
     </row>
@@ -28418,7 +28418,7 @@
         <v>45769</v>
       </c>
       <c r="B1391">
-        <v>424.08080000000001</v>
+        <v>424.08170000000001</v>
       </c>
       <c r="C1391">
         <v>1934</v>
@@ -28438,7 +28438,7 @@
         <v>45770</v>
       </c>
       <c r="B1392">
-        <v>426.30739999999997</v>
+        <v>426.3098</v>
       </c>
       <c r="C1392">
         <v>1934</v>
@@ -28458,7 +28458,7 @@
         <v>45771</v>
       </c>
       <c r="B1393">
-        <v>428.37020000000001</v>
+        <v>428.37360000000001</v>
       </c>
       <c r="C1393">
         <v>1934</v>
@@ -28478,7 +28478,7 @@
         <v>45772</v>
       </c>
       <c r="B1394">
-        <v>430.85829999999999</v>
+        <v>430.86279999999999</v>
       </c>
       <c r="C1394">
         <v>2041</v>
@@ -28498,7 +28498,7 @@
         <v>45775</v>
       </c>
       <c r="B1395">
-        <v>440.11189999999999</v>
+        <v>440.1164</v>
       </c>
       <c r="C1395">
         <v>2041</v>
@@ -28518,7 +28518,7 @@
         <v>45776</v>
       </c>
       <c r="B1396">
-        <v>443.05770000000001</v>
+        <v>443.06229999999999</v>
       </c>
       <c r="C1396">
         <v>2041</v>
@@ -28538,7 +28538,7 @@
         <v>45777</v>
       </c>
       <c r="B1397">
-        <v>446.48349999999999</v>
+        <v>446.488</v>
       </c>
       <c r="C1397">
         <v>2041</v>
@@ -28558,7 +28558,7 @@
         <v>45778</v>
       </c>
       <c r="B1398">
-        <v>451.06439999999998</v>
+        <v>451.06909999999999</v>
       </c>
       <c r="C1398">
         <v>2041</v>
@@ -28578,7 +28578,7 @@
         <v>45779</v>
       </c>
       <c r="B1399">
-        <v>455.56169999999997</v>
+        <v>455.56639999999999</v>
       </c>
       <c r="C1399">
         <v>2145</v>
@@ -28598,7 +28598,7 @@
         <v>45782</v>
       </c>
       <c r="B1400">
-        <v>468.04129999999998</v>
+        <v>468.04610000000002</v>
       </c>
       <c r="C1400">
         <v>2145</v>
@@ -28618,7 +28618,7 @@
         <v>45783</v>
       </c>
       <c r="B1401">
-        <v>470.54739999999998</v>
+        <v>470.5521</v>
       </c>
       <c r="C1401">
         <v>2145</v>
@@ -28638,7 +28638,7 @@
         <v>45784</v>
       </c>
       <c r="B1402">
-        <v>472.84609999999998</v>
+        <v>472.851</v>
       </c>
       <c r="C1402">
         <v>2145</v>
@@ -29578,7 +29578,7 @@
         <v>45849</v>
       </c>
       <c r="B1449">
-        <v>705.55970000000002</v>
+        <v>705.5598</v>
       </c>
       <c r="C1449">
         <v>3052</v>
@@ -29658,13 +29658,13 @@
         <v>45855</v>
       </c>
       <c r="B1453">
-        <v>726.25400000000002</v>
+        <v>727.01760000000002</v>
       </c>
       <c r="C1453">
         <v>3052</v>
       </c>
       <c r="D1453">
-        <v>2.7837000000000001</v>
+        <v>2.8287</v>
       </c>
       <c r="E1453">
         <v>139.12729999999999</v>
@@ -29678,16 +29678,16 @@
         <v>45856</v>
       </c>
       <c r="B1454">
-        <v>729.52409999999998</v>
+        <v>730.27149999999995</v>
       </c>
       <c r="C1454">
-        <v>3052</v>
+        <v>3075</v>
       </c>
       <c r="D1454">
-        <v>2.8287</v>
+        <v>2.8736999999999999</v>
       </c>
       <c r="E1454">
-        <v>139.77619999999999</v>
+        <v>139.7706</v>
       </c>
       <c r="F1454">
         <v>77.134900000000002</v>
@@ -29698,19 +29698,99 @@
         <v>45859</v>
       </c>
       <c r="B1455">
-        <v>734.0104</v>
+        <v>741.7722</v>
       </c>
       <c r="C1455">
-        <v>3052</v>
+        <v>3075</v>
       </c>
       <c r="D1455">
-        <v>2.8736999999999999</v>
+        <v>3.0085999999999999</v>
       </c>
       <c r="E1455">
-        <v>140.87899999999999</v>
+        <v>142.58779999999999</v>
       </c>
       <c r="F1455">
-        <v>77.606200000000001</v>
+        <v>78.606200000000001</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1456" s="2">
+        <v>45860</v>
+      </c>
+      <c r="B1456">
+        <v>745.10479999999995</v>
+      </c>
+      <c r="C1456">
+        <v>3075</v>
+      </c>
+      <c r="D1456">
+        <v>3.0579999999999998</v>
+      </c>
+      <c r="E1456">
+        <v>143.21270000000001</v>
+      </c>
+      <c r="F1456">
+        <v>79.211299999999994</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1457" s="2">
+        <v>45861</v>
+      </c>
+      <c r="B1457">
+        <v>748.33460000000002</v>
+      </c>
+      <c r="C1457">
+        <v>3075</v>
+      </c>
+      <c r="D1457">
+        <v>3.0579999999999998</v>
+      </c>
+      <c r="E1457">
+        <v>143.8321</v>
+      </c>
+      <c r="F1457">
+        <v>79.651799999999994</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1458" s="2">
+        <v>45862</v>
+      </c>
+      <c r="B1458">
+        <v>748.33460000000002</v>
+      </c>
+      <c r="C1458">
+        <v>3075</v>
+      </c>
+      <c r="D1458">
+        <v>3.0579999999999998</v>
+      </c>
+      <c r="E1458">
+        <v>143.8321</v>
+      </c>
+      <c r="F1458">
+        <v>79.651799999999994</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1459" s="2">
+        <v>45863</v>
+      </c>
+      <c r="B1459">
+        <v>748.33460000000002</v>
+      </c>
+      <c r="C1459">
+        <v>3075</v>
+      </c>
+      <c r="D1459">
+        <v>3.0579999999999998</v>
+      </c>
+      <c r="E1459">
+        <v>143.8321</v>
+      </c>
+      <c r="F1459">
+        <v>79.651799999999994</v>
       </c>
     </row>
   </sheetData>
@@ -29720,10 +29800,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CC2F69-7C8C-4154-8046-9289F76718B0}">
-  <dimension ref="A1:C1193"/>
+  <dimension ref="A1:C1197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1142" workbookViewId="0">
-      <selection activeCell="C1201" sqref="C1201:C1202"/>
+    <sheetView tabSelected="1" topLeftCell="A1161" workbookViewId="0">
+      <selection activeCell="G1187" sqref="G1187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29777,14 +29857,14 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=1187")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=1191")</f>
         <v>44197</v>
       </c>
       <c r="B7">
         <v>32.590000000000003</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1187")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=1191")</f>
         <v>19.074999999999999</v>
       </c>
     </row>
@@ -42828,10 +42908,54 @@
         <v>45859</v>
       </c>
       <c r="B1193">
-        <v>69.62</v>
+        <v>69.47</v>
       </c>
       <c r="C1193">
-        <v>33.950000000000003</v>
+        <v>33.409999999999997</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1194" s="2">
+        <v>45860</v>
+      </c>
+      <c r="B1194">
+        <v>68.75</v>
+      </c>
+      <c r="C1194">
+        <v>33.325000000000003</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1195" s="2">
+        <v>45861</v>
+      </c>
+      <c r="B1195">
+        <v>69</v>
+      </c>
+      <c r="C1195">
+        <v>32.65</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1196" s="2">
+        <v>45862</v>
+      </c>
+      <c r="B1196">
+        <v>70.5</v>
+      </c>
+      <c r="C1196">
+        <v>32.25</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1197" s="2">
+        <v>45863</v>
+      </c>
+      <c r="B1197">
+        <v>70.63</v>
+      </c>
+      <c r="C1197">
+        <v>32.549999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>